<commit_message>
multiplication tables work, need to add font
</commit_message>
<xml_diff>
--- a/12_ExcelSpreadsheets/multiTables.xlsx
+++ b/12_ExcelSpreadsheets/multiTables.xlsx
@@ -383,40 +383,232 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I2" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
+      <c r="B3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" t="n">
+        <v>12</v>
+      </c>
+      <c r="H3" t="n">
+        <v>14</v>
+      </c>
+      <c r="I3" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
         <v>3</v>
       </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9</v>
+      </c>
+      <c r="E4" t="n">
+        <v>12</v>
+      </c>
+      <c r="F4" t="n">
+        <v>15</v>
+      </c>
+      <c r="G4" t="n">
+        <v>18</v>
+      </c>
+      <c r="H4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I4" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
         <v>4</v>
       </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" t="n">
+        <v>16</v>
+      </c>
+      <c r="F5" t="n">
+        <v>20</v>
+      </c>
+      <c r="G5" t="n">
+        <v>24</v>
+      </c>
+      <c r="H5" t="n">
+        <v>28</v>
+      </c>
+      <c r="I5" t="n">
+        <v>32</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
         <v>5</v>
       </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" t="n">
+        <v>15</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" t="n">
+        <v>25</v>
+      </c>
+      <c r="G6" t="n">
+        <v>30</v>
+      </c>
+      <c r="H6" t="n">
+        <v>35</v>
+      </c>
+      <c r="I6" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
         <v>6</v>
       </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" t="n">
+        <v>24</v>
+      </c>
+      <c r="F7" t="n">
+        <v>30</v>
+      </c>
+      <c r="G7" t="n">
+        <v>36</v>
+      </c>
+      <c r="H7" t="n">
+        <v>42</v>
+      </c>
+      <c r="I7" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
         <v>7</v>
       </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>14</v>
+      </c>
+      <c r="D8" t="n">
+        <v>21</v>
+      </c>
+      <c r="E8" t="n">
+        <v>28</v>
+      </c>
+      <c r="F8" t="n">
+        <v>35</v>
+      </c>
+      <c r="G8" t="n">
+        <v>42</v>
+      </c>
+      <c r="H8" t="n">
+        <v>49</v>
+      </c>
+      <c r="I8" t="n">
+        <v>56</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
         <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16</v>
+      </c>
+      <c r="D9" t="n">
+        <v>24</v>
+      </c>
+      <c r="E9" t="n">
+        <v>32</v>
+      </c>
+      <c r="F9" t="n">
+        <v>40</v>
+      </c>
+      <c r="G9" t="n">
+        <v>48</v>
+      </c>
+      <c r="H9" t="n">
+        <v>56</v>
+      </c>
+      <c r="I9" t="n">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added styling to multiplication table project
</commit_message>
<xml_diff>
--- a/12_ExcelSpreadsheets/multiTables.xlsx
+++ b/12_ExcelSpreadsheets/multiTables.xlsx
@@ -17,13 +17,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -345,7 +350,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -354,33 +359,45 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" t="n">
+      <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" t="n">
+      <c r="C1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D1" t="n">
+      <c r="D1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E1" t="n">
+      <c r="E1" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F1" t="n">
+      <c r="F1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="G1" t="n">
+      <c r="G1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H1" t="n">
+      <c r="H1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I1" t="n">
+      <c r="I1" s="1" t="n">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" t="n">
@@ -407,9 +424,21 @@
       <c r="I2" t="n">
         <v>8</v>
       </c>
+      <c r="J2" t="n">
+        <v>9</v>
+      </c>
+      <c r="K2" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2" t="n">
+        <v>11</v>
+      </c>
+      <c r="M2" t="n">
+        <v>12</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="B3" t="n">
@@ -436,9 +465,21 @@
       <c r="I3" t="n">
         <v>16</v>
       </c>
+      <c r="J3" t="n">
+        <v>18</v>
+      </c>
+      <c r="K3" t="n">
+        <v>20</v>
+      </c>
+      <c r="L3" t="n">
+        <v>22</v>
+      </c>
+      <c r="M3" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B4" t="n">
@@ -465,9 +506,21 @@
       <c r="I4" t="n">
         <v>24</v>
       </c>
+      <c r="J4" t="n">
+        <v>27</v>
+      </c>
+      <c r="K4" t="n">
+        <v>30</v>
+      </c>
+      <c r="L4" t="n">
+        <v>33</v>
+      </c>
+      <c r="M4" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B5" t="n">
@@ -494,9 +547,21 @@
       <c r="I5" t="n">
         <v>32</v>
       </c>
+      <c r="J5" t="n">
+        <v>36</v>
+      </c>
+      <c r="K5" t="n">
+        <v>40</v>
+      </c>
+      <c r="L5" t="n">
+        <v>44</v>
+      </c>
+      <c r="M5" t="n">
+        <v>48</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B6" t="n">
@@ -523,9 +588,21 @@
       <c r="I6" t="n">
         <v>40</v>
       </c>
+      <c r="J6" t="n">
+        <v>45</v>
+      </c>
+      <c r="K6" t="n">
+        <v>50</v>
+      </c>
+      <c r="L6" t="n">
+        <v>55</v>
+      </c>
+      <c r="M6" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B7" t="n">
@@ -552,9 +629,21 @@
       <c r="I7" t="n">
         <v>48</v>
       </c>
+      <c r="J7" t="n">
+        <v>54</v>
+      </c>
+      <c r="K7" t="n">
+        <v>60</v>
+      </c>
+      <c r="L7" t="n">
+        <v>66</v>
+      </c>
+      <c r="M7" t="n">
+        <v>72</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B8" t="n">
@@ -581,9 +670,21 @@
       <c r="I8" t="n">
         <v>56</v>
       </c>
+      <c r="J8" t="n">
+        <v>63</v>
+      </c>
+      <c r="K8" t="n">
+        <v>70</v>
+      </c>
+      <c r="L8" t="n">
+        <v>77</v>
+      </c>
+      <c r="M8" t="n">
+        <v>84</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
+      <c r="A9" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B9" t="n">
@@ -609,6 +710,182 @@
       </c>
       <c r="I9" t="n">
         <v>64</v>
+      </c>
+      <c r="J9" t="n">
+        <v>72</v>
+      </c>
+      <c r="K9" t="n">
+        <v>80</v>
+      </c>
+      <c r="L9" t="n">
+        <v>88</v>
+      </c>
+      <c r="M9" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>18</v>
+      </c>
+      <c r="D10" t="n">
+        <v>27</v>
+      </c>
+      <c r="E10" t="n">
+        <v>36</v>
+      </c>
+      <c r="F10" t="n">
+        <v>45</v>
+      </c>
+      <c r="G10" t="n">
+        <v>54</v>
+      </c>
+      <c r="H10" t="n">
+        <v>63</v>
+      </c>
+      <c r="I10" t="n">
+        <v>72</v>
+      </c>
+      <c r="J10" t="n">
+        <v>81</v>
+      </c>
+      <c r="K10" t="n">
+        <v>90</v>
+      </c>
+      <c r="L10" t="n">
+        <v>99</v>
+      </c>
+      <c r="M10" t="n">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>20</v>
+      </c>
+      <c r="D11" t="n">
+        <v>30</v>
+      </c>
+      <c r="E11" t="n">
+        <v>40</v>
+      </c>
+      <c r="F11" t="n">
+        <v>50</v>
+      </c>
+      <c r="G11" t="n">
+        <v>60</v>
+      </c>
+      <c r="H11" t="n">
+        <v>70</v>
+      </c>
+      <c r="I11" t="n">
+        <v>80</v>
+      </c>
+      <c r="J11" t="n">
+        <v>90</v>
+      </c>
+      <c r="K11" t="n">
+        <v>100</v>
+      </c>
+      <c r="L11" t="n">
+        <v>110</v>
+      </c>
+      <c r="M11" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>22</v>
+      </c>
+      <c r="D12" t="n">
+        <v>33</v>
+      </c>
+      <c r="E12" t="n">
+        <v>44</v>
+      </c>
+      <c r="F12" t="n">
+        <v>55</v>
+      </c>
+      <c r="G12" t="n">
+        <v>66</v>
+      </c>
+      <c r="H12" t="n">
+        <v>77</v>
+      </c>
+      <c r="I12" t="n">
+        <v>88</v>
+      </c>
+      <c r="J12" t="n">
+        <v>99</v>
+      </c>
+      <c r="K12" t="n">
+        <v>110</v>
+      </c>
+      <c r="L12" t="n">
+        <v>121</v>
+      </c>
+      <c r="M12" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>24</v>
+      </c>
+      <c r="D13" t="n">
+        <v>36</v>
+      </c>
+      <c r="E13" t="n">
+        <v>48</v>
+      </c>
+      <c r="F13" t="n">
+        <v>60</v>
+      </c>
+      <c r="G13" t="n">
+        <v>72</v>
+      </c>
+      <c r="H13" t="n">
+        <v>84</v>
+      </c>
+      <c r="I13" t="n">
+        <v>96</v>
+      </c>
+      <c r="J13" t="n">
+        <v>108</v>
+      </c>
+      <c r="K13" t="n">
+        <v>120</v>
+      </c>
+      <c r="L13" t="n">
+        <v>132</v>
+      </c>
+      <c r="M13" t="n">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>